<commit_message>
Evaluation beendet an Spring + GoKit
</commit_message>
<xml_diff>
--- a/Sonstiges/MFEM-Beispiel-GoKit.xlsx
+++ b/Sonstiges/MFEM-Beispiel-GoKit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="QUT-GQM" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="102">
   <si>
     <t>1: Installation / Einrichtung</t>
   </si>
@@ -131,9 +131,6 @@
 (0.0 - 1.0)</t>
   </si>
   <si>
-    <t>Progressivität</t>
-  </si>
-  <si>
     <t>Aktive Community</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>Ist der Service leichtgewichtig?</t>
   </si>
   <si>
-    <t>Messung Heap Size: Kleiner 100MB</t>
-  </si>
-  <si>
     <t>Lässt sich automatisiert ein Build vom Service erstellen</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>Wie lange wird ein Support gewährleistet?</t>
   </si>
   <si>
-    <t>Länge vom Support in Jahren pro Major Release</t>
-  </si>
-  <si>
     <t>Gibt es vom Hersteller Support</t>
   </si>
   <si>
@@ -267,12 +258,6 @@
     <t>Stehen große Firmen dahinter?</t>
   </si>
   <si>
-    <t>Anzahl Firmen über 1000 MA</t>
-  </si>
-  <si>
-    <t>Anzahl Firmen über 100 MA</t>
-  </si>
-  <si>
     <t>Wie viele Benutzer gibt es</t>
   </si>
   <si>
@@ -285,16 +270,73 @@
     <t>Latenz Antwort bei Messung an Endpunkt ohne Logik</t>
   </si>
   <si>
-    <t>Bleibt der Service bei Lastspitzen verfügbar?</t>
-  </si>
-  <si>
-    <t>Druchsatz bei 50.000 Anfragen mit 500 echt parallelen Clients in Anfragen/Sek</t>
-  </si>
-  <si>
-    <t>Stabile und kurze Reakionszeit</t>
-  </si>
-  <si>
-    <t>Fehlerrate bei 50.000 Anfragen mit 500 echt parallelen Clients in %</t>
+    <t>Kurze Reakionszeit</t>
+  </si>
+  <si>
+    <t>Kann der Service Lastspitzen aushalten und bewältigen?</t>
+  </si>
+  <si>
+    <t>Druchsatz bei 100.000 Anfragen mit 255 echt parallelen Clients in Anfragen/Sek</t>
+  </si>
+  <si>
+    <t>Messung Heap Size unter Last: Kleiner 100MB</t>
+  </si>
+  <si>
+    <t>Länge vom Support in Monaten pro Major Release</t>
+  </si>
+  <si>
+    <t>Firmen über 1000 MA</t>
+  </si>
+  <si>
+    <t>Firmen über 100 MA</t>
+  </si>
+  <si>
+    <t>31MB</t>
+  </si>
+  <si>
+    <t>27.625,2 Anfragen/sec</t>
+  </si>
+  <si>
+    <t>9ms</t>
+  </si>
+  <si>
+    <t>unklar</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>Noch nicht v1</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Zukunftssicherheit</t>
+  </si>
+  <si>
+    <t>leicht umsetzbar</t>
+  </si>
+  <si>
+    <t>Verfügbar</t>
+  </si>
+  <si>
+    <t>Sehr gut</t>
+  </si>
+  <si>
+    <t>manuell</t>
+  </si>
+  <si>
+    <t>enthalten</t>
+  </si>
+  <si>
+    <t>schwer umsetzbar</t>
+  </si>
+  <si>
+    <t>gut</t>
+  </si>
+  <si>
+    <t>Einfach</t>
   </si>
 </sst>
 </file>
@@ -685,7 +727,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -708,36 +750,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -748,9 +760,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -813,17 +822,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -963,7 +1014,7 @@
                   <c:v>Wartbarkeit</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Progressivität</c:v>
+                  <c:v>Zukunftssicherheit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -975,22 +1026,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.568181818181818</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0.558571428571429</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0.285714285714286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0.104166666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1004,11 +1055,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1758300448"/>
-        <c:axId val="1857364624"/>
+        <c:axId val="2063944416"/>
+        <c:axId val="2063946048"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="1758300448"/>
+        <c:axId val="2063944416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1102,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1857364624"/>
+        <c:crossAx val="2063946048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1059,7 +1110,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1857364624"/>
+        <c:axId val="2063946048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1110,7 +1161,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1758300448"/>
+        <c:crossAx val="2063944416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2002,21 +2053,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="36" customWidth="1"/>
-    <col min="3" max="3" width="42.83203125" style="55" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="36" customWidth="1"/>
-    <col min="5" max="5" width="37.33203125" style="55" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="31" style="55" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="25" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" style="42" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" style="42" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="31" style="42" customWidth="1"/>
     <col min="8" max="8" width="24.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
@@ -2025,54 +2076,54 @@
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="42" t="s">
+      <c r="E1" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="49" t="s">
+      <c r="G1" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="23">
         <v>1</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="23">
         <v>1</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="39">
+        <v>1</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="50">
-        <v>1</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="37">
+      <c r="H2" s="26">
         <v>0.5</v>
       </c>
       <c r="I2" s="1">
@@ -2081,415 +2132,425 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="29">
+      <c r="A3" s="49"/>
+      <c r="B3" s="46">
         <v>2</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="23">
         <v>2</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="39">
+        <v>2</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="50">
-        <v>2</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="37">
+      <c r="H3" s="26">
         <v>0.5</v>
       </c>
       <c r="I3" s="2">
         <f>IFERROR(VLOOKUP($F3,Evaluation!C:F,4,FALSE),0)*H3</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="35">
+      <c r="A4" s="53"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="24">
         <v>3</v>
       </c>
-      <c r="E4" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="50">
+      <c r="E4" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="39">
         <v>3</v>
       </c>
-      <c r="G4" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="38">
+      <c r="G4" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="27">
         <v>0.25</v>
       </c>
       <c r="I4" s="2">
         <f>IFERROR(VLOOKUP($F4,Evaluation!C:F,4,FALSE),0)*H4</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="29">
+      <c r="A5" s="53"/>
+      <c r="B5" s="46">
         <v>3</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="23">
         <v>4</v>
       </c>
-      <c r="E5" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="50">
+      <c r="E5" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="39">
         <v>4</v>
       </c>
-      <c r="G5" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="38">
+      <c r="G5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="27">
         <v>1</v>
       </c>
       <c r="I5" s="2">
         <f>IFERROR(VLOOKUP($F5,Evaluation!C:F,4,FALSE),0)*H5</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="34">
+      <c r="A6" s="53"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="23">
         <v>5</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="39">
+        <v>5</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="50">
-        <v>5</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="38">
+      <c r="H6" s="27">
         <v>0.25</v>
       </c>
       <c r="I6" s="2">
         <f>IFERROR(VLOOKUP($F6,Evaluation!C:F,4,FALSE),0)*H6</f>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="35">
+      <c r="A7" s="53"/>
+      <c r="B7" s="24">
         <v>4</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="24">
         <v>6</v>
       </c>
-      <c r="E7" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="50">
+      <c r="E7" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="39">
         <v>6</v>
       </c>
-      <c r="G7" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="38">
+      <c r="G7" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="27">
         <v>0.25</v>
       </c>
       <c r="I7" s="2">
         <f>IFERROR(VLOOKUP($F7,Evaluation!C:F,4,FALSE),0)*H7</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="18">
         <v>5</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="34">
+      <c r="C8" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="23">
         <v>7</v>
       </c>
-      <c r="E8" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="50">
+      <c r="E8" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="39">
         <v>7</v>
       </c>
-      <c r="G8" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" s="38">
+      <c r="G8" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="27">
         <v>0.5</v>
       </c>
       <c r="I8" s="2">
         <f>IFERROR(VLOOKUP($F8,Evaluation!C:F,4,FALSE),0)*H8</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="29">
+      <c r="A9" s="48"/>
+      <c r="B9" s="23">
+        <v>6</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="20">
         <v>8</v>
       </c>
-      <c r="E9" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="50">
+      <c r="E9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="39">
         <v>8</v>
       </c>
-      <c r="G9" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" s="38">
+      <c r="G9" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="27">
         <v>0.5</v>
       </c>
       <c r="I9" s="2">
         <f>IFERROR(VLOOKUP($F9,Evaluation!C:F,4,FALSE),0)*H9</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="34">
-        <v>6</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="50">
+      <c r="A10" s="49"/>
+      <c r="B10" s="24">
+        <v>7</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="24">
         <v>9</v>
       </c>
-      <c r="G10" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="38">
-        <v>0.5</v>
+      <c r="E10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="39">
+        <v>9</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0.25</v>
       </c>
       <c r="I10" s="2">
         <f>IFERROR(VLOOKUP($F10,Evaluation!C:F,4,FALSE),0)*H10</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="35">
-        <v>7</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="35">
-        <v>9</v>
-      </c>
-      <c r="E11" s="33" t="s">
+      <c r="A11" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="46">
+        <v>8</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="24">
+        <v>10</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="50">
+      <c r="F11" s="39">
         <v>10</v>
       </c>
-      <c r="G11" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="38">
-        <v>0.25</v>
+      <c r="G11" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="27">
+        <v>1</v>
       </c>
       <c r="I11" s="2">
         <f>IFERROR(VLOOKUP($F11,Evaluation!C:F,4,FALSE),0)*H11</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="29">
-        <v>8</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="35">
-        <v>10</v>
-      </c>
-      <c r="E12" s="33" t="s">
+      <c r="A12" s="48"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="23">
+        <v>11</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="39">
+        <v>11</v>
+      </c>
+      <c r="G12" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="50">
-        <v>11</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="38">
-        <v>1</v>
+      <c r="H12" s="27">
+        <v>0.25</v>
       </c>
       <c r="I12" s="2">
         <f>IFERROR(VLOOKUP($F12,Evaluation!C:F,4,FALSE),0)*H12</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="34">
-        <v>11</v>
-      </c>
-      <c r="E13" s="33" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="46">
+        <v>9</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="46">
+        <v>12</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="39">
+        <v>12</v>
+      </c>
+      <c r="G13" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="50">
-        <v>12</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="38">
+      <c r="H13" s="27">
         <v>0.25</v>
       </c>
       <c r="I13" s="2">
         <f>IFERROR(VLOOKUP($F13,Evaluation!C:F,4,FALSE),0)*H13</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="29">
-        <v>9</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="29">
-        <v>12</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="50">
+      <c r="A14" s="48"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="39">
         <v>13</v>
       </c>
-      <c r="G14" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="38">
+      <c r="G14" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="27">
         <v>0.25</v>
       </c>
       <c r="I14" s="2">
         <f>IFERROR(VLOOKUP($F14,Evaluation!C:F,4,FALSE),0)*H14</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="50">
+      <c r="A15" s="48"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="23">
+        <v>13</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="39">
         <v>14</v>
       </c>
-      <c r="G15" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="38">
+      <c r="G15" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="27">
         <v>0.25</v>
       </c>
       <c r="I15" s="2">
         <f>IFERROR(VLOOKUP($F15,Evaluation!C:F,4,FALSE),0)*H15</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="34">
-        <v>13</v>
-      </c>
-      <c r="E16" s="33" t="s">
+      <c r="A16" s="48"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="23">
+        <v>14</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="50">
+      <c r="F16" s="39">
         <v>15</v>
       </c>
-      <c r="G16" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="38">
-        <v>0.25</v>
+      <c r="G16" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="27">
+        <v>0.5</v>
       </c>
       <c r="I16" s="2">
         <f>IFERROR(VLOOKUP($F16,Evaluation!C:F,4,FALSE),0)*H16</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="34">
-        <v>14</v>
-      </c>
-      <c r="E17" s="33" t="s">
+      <c r="A17" s="49"/>
+      <c r="B17" s="24">
+        <v>10</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="24">
+        <v>15</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="50">
+      <c r="F17" s="39">
         <v>16</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="G17" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="38">
-        <v>0.5</v>
+      <c r="H17" s="27">
+        <v>1</v>
       </c>
       <c r="I17" s="2">
         <f>IFERROR(VLOOKUP($F17,Evaluation!C:F,4,FALSE),0)*H17</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="35">
-        <v>10</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="35">
-        <v>15</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="50">
+      <c r="A18" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="24">
+        <v>11</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="24">
+        <v>16</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="39">
         <v>17</v>
       </c>
-      <c r="G18" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="38">
-        <v>1</v>
+      <c r="G18" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="27">
+        <v>0.5</v>
       </c>
       <c r="I18" s="2">
         <f>IFERROR(VLOOKUP($F18,Evaluation!C:F,4,FALSE),0)*H18</f>
@@ -2497,111 +2558,109 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="35">
-        <v>11</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="35">
-        <v>16</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="50">
+      <c r="A19" s="49"/>
+      <c r="B19" s="23">
+        <v>12</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="23">
+        <v>17</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="39">
         <v>18</v>
       </c>
-      <c r="G19" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" s="38">
-        <v>0.5</v>
+      <c r="G19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="27">
+        <v>1</v>
       </c>
       <c r="I19" s="2">
         <f>IFERROR(VLOOKUP($F19,Evaluation!C:F,4,FALSE),0)*H19</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="34">
-        <v>12</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="34">
-        <v>17</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="50">
+      <c r="A20" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="46">
+        <v>13</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="24">
+        <v>18</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="39">
         <v>19</v>
       </c>
-      <c r="G20" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="H20" s="38">
-        <v>1</v>
+      <c r="G20" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="27">
+        <v>0.5</v>
       </c>
       <c r="I20" s="2">
         <f>IFERROR(VLOOKUP($F20,Evaluation!C:F,4,FALSE),0)*H20</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="29">
-        <v>13</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="35">
-        <v>18</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="50">
+      <c r="A21" s="48"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="23">
+        <v>19</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="39">
         <v>20</v>
       </c>
-      <c r="G21" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" s="38">
+      <c r="G21" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="27">
         <v>0.5</v>
       </c>
       <c r="I21" s="2">
         <f>IFERROR(VLOOKUP($F21,Evaluation!C:F,4,FALSE),0)*H21</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="34">
-        <v>19</v>
-      </c>
-      <c r="E22" s="33" t="s">
+      <c r="A22" s="48"/>
+      <c r="B22" s="46">
+        <v>14</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="23">
+        <v>20</v>
+      </c>
+      <c r="E22" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="50">
+      <c r="F22" s="39">
         <v>21</v>
       </c>
-      <c r="G22" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="H22" s="38">
-        <v>0.5</v>
+      <c r="G22" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="27">
+        <v>0.25</v>
       </c>
       <c r="I22" s="2">
         <f>IFERROR(VLOOKUP($F22,Evaluation!C:F,4,FALSE),0)*H22</f>
@@ -2609,26 +2668,22 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="29">
-        <v>14</v>
-      </c>
-      <c r="C23" s="30" t="s">
+      <c r="A23" s="49"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="23">
+        <v>21</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="34">
-        <v>20</v>
-      </c>
-      <c r="E23" s="33" t="s">
+      <c r="F23" s="39">
+        <v>22</v>
+      </c>
+      <c r="G23" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="50">
-        <v>22</v>
-      </c>
-      <c r="G23" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="H23" s="38">
+      <c r="H23" s="27">
         <v>0.5</v>
       </c>
       <c r="I23" s="2">
@@ -2637,23 +2692,29 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="34">
-        <v>21</v>
-      </c>
-      <c r="E24" s="33" t="s">
+      <c r="A24" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="46">
+        <v>15</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="24">
+        <v>22</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="39">
+        <v>23</v>
+      </c>
+      <c r="G24" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="50">
-        <v>23</v>
-      </c>
-      <c r="G24" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="H24" s="38">
-        <v>0.25</v>
+      <c r="H24" s="27">
+        <v>0.5</v>
       </c>
       <c r="I24" s="2">
         <f>IFERROR(VLOOKUP($F24,Evaluation!C:F,4,FALSE),0)*H24</f>
@@ -2661,29 +2722,23 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="29">
-        <v>15</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="35">
-        <v>22</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="50">
+      <c r="A25" s="48"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="46">
+        <v>23</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="39">
         <v>24</v>
       </c>
-      <c r="G25" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="H25" s="38">
-        <v>0.5</v>
+      <c r="G25" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="27">
+        <v>0.1</v>
       </c>
       <c r="I25" s="2">
         <f>IFERROR(VLOOKUP($F25,Evaluation!C:F,4,FALSE),0)*H25</f>
@@ -2691,22 +2746,18 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="29">
-        <v>23</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="50">
+      <c r="A26" s="48"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="39">
         <v>25</v>
       </c>
-      <c r="G26" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" s="38">
+      <c r="G26" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="27">
         <v>0.1</v>
       </c>
       <c r="I26" s="2">
@@ -2715,44 +2766,38 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="50">
+      <c r="A27" s="49"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="24">
+        <v>24</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="39">
         <v>26</v>
       </c>
-      <c r="G27" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="H27" s="38">
-        <v>0.1</v>
+      <c r="G27" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="27">
+        <v>0.5</v>
       </c>
       <c r="I27" s="2">
         <f>IFERROR(VLOOKUP($F27,Evaluation!C:F,4,FALSE),0)*H27</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="35">
-        <v>24</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="50">
-        <v>27</v>
-      </c>
-      <c r="G28" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="H28" s="38">
-        <v>0.5</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="27"/>
       <c r="I28" s="2">
         <f>IFERROR(VLOOKUP($F28,Evaluation!C:F,4,FALSE),0)*H28</f>
         <v>0</v>
@@ -2760,13 +2805,13 @@
     </row>
     <row r="29" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="38"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="2">
         <f>IFERROR(VLOOKUP($F29,Evaluation!C:F,4,FALSE),0)*H29</f>
         <v>0</v>
@@ -2774,13 +2819,13 @@
     </row>
     <row r="30" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="38"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="2">
         <f>IFERROR(VLOOKUP($F30,Evaluation!C:F,4,FALSE),0)*H30</f>
         <v>0</v>
@@ -2788,13 +2833,13 @@
     </row>
     <row r="31" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="38"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="27"/>
       <c r="I31" s="2">
         <f>IFERROR(VLOOKUP($F31,Evaluation!C:F,4,FALSE),0)*H31</f>
         <v>0</v>
@@ -2802,13 +2847,13 @@
     </row>
     <row r="32" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="38"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="27"/>
       <c r="I32" s="2">
         <f>IFERROR(VLOOKUP($F32,Evaluation!C:F,4,FALSE),0)*H32</f>
         <v>0</v>
@@ -2816,13 +2861,13 @@
     </row>
     <row r="33" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="38"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="27"/>
       <c r="I33" s="2">
         <f>IFERROR(VLOOKUP($F33,Evaluation!C:F,4,FALSE),0)*H33</f>
         <v>0</v>
@@ -2830,13 +2875,13 @@
     </row>
     <row r="34" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="38"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="27"/>
       <c r="I34" s="2">
         <f>IFERROR(VLOOKUP($F34,Evaluation!C:F,4,FALSE),0)*H34</f>
         <v>0</v>
@@ -2844,13 +2889,13 @@
     </row>
     <row r="35" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="38"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="27"/>
       <c r="I35" s="2">
         <f>IFERROR(VLOOKUP($F35,Evaluation!C:F,4,FALSE),0)*H35</f>
         <v>0</v>
@@ -2858,13 +2903,13 @@
     </row>
     <row r="36" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="38"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="27"/>
       <c r="I36" s="2">
         <f>IFERROR(VLOOKUP($F36,Evaluation!C:F,4,FALSE),0)*H36</f>
         <v>0</v>
@@ -2872,13 +2917,13 @@
     </row>
     <row r="37" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="38"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="27"/>
       <c r="I37" s="2">
         <f>IFERROR(VLOOKUP($F37,Evaluation!C:F,4,FALSE),0)*H37</f>
         <v>0</v>
@@ -2886,13 +2931,13 @@
     </row>
     <row r="38" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="38"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="27"/>
       <c r="I38" s="2">
         <f>IFERROR(VLOOKUP($F38,Evaluation!C:F,4,FALSE),0)*H38</f>
         <v>0</v>
@@ -2900,13 +2945,13 @@
     </row>
     <row r="39" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="38"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="27"/>
       <c r="I39" s="2">
         <f>IFERROR(VLOOKUP($F39,Evaluation!C:F,4,FALSE),0)*H39</f>
         <v>0</v>
@@ -2914,13 +2959,13 @@
     </row>
     <row r="40" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="38"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="27"/>
       <c r="I40" s="2">
         <f>IFERROR(VLOOKUP($F40,Evaluation!C:F,4,FALSE),0)*H40</f>
         <v>0</v>
@@ -2928,13 +2973,13 @@
     </row>
     <row r="41" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="38"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="27"/>
       <c r="I41" s="2">
         <f>IFERROR(VLOOKUP($F41,Evaluation!C:F,4,FALSE),0)*H41</f>
         <v>0</v>
@@ -2942,76 +2987,58 @@
     </row>
     <row r="42" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="38"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="27"/>
       <c r="I42" s="2">
         <f>IFERROR(VLOOKUP($F42,Evaluation!C:F,4,FALSE),0)*H42</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="2">
+    <row r="43" spans="1:9" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="32"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="3">
         <f>IFERROR(VLOOKUP($F43,Evaluation!C:F,4,FALSE),0)*H43</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="3">
-        <f>IFERROR(VLOOKUP($F44,Evaluation!C:F,4,FALSE),0)*H44</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A21:A24"/>
+  <mergeCells count="24">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A17"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3021,8 +3048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3034,7 +3061,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -3046,136 +3073,148 @@
       <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>IFERROR(VLOOKUP($C2,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (Verfügbar, leicht umsetzbar, schwer umsetzbar)</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="46"/>
+      <c r="E2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="35">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="str">
         <f>IFERROR(VLOOKUP($C3,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (Verfügbar, leicht umsetzbar, schwer umsetzbar)</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="47"/>
+      <c r="E3" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="17"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>IFERROR(VLOOKUP($C4,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (sehr gut, gut, schlecht)</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="47"/>
+      <c r="E4" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="9"/>
       <c r="D5" s="2" t="str">
         <f>IFERROR(VLOOKUP($C5,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="47"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="17"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="9"/>
       <c r="D6" s="2" t="str">
         <f>IFERROR(VLOOKUP($C6,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="47"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
-      <c r="B7" s="17"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="9"/>
       <c r="D7" s="2" t="str">
         <f>IFERROR(VLOOKUP($C7,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="47"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="17"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="9"/>
       <c r="D8" s="2" t="str">
         <f>IFERROR(VLOOKUP($C8,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="47"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="9"/>
       <c r="D9" s="2" t="str">
         <f>IFERROR(VLOOKUP($C9,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="47"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="9"/>
       <c r="D10" s="2" t="str">
         <f>IFERROR(VLOOKUP($C10,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="47"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="10"/>
       <c r="D11" s="3" t="str">
         <f>IFERROR(VLOOKUP($C11,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="48"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="16" t="s">
+      <c r="A12" s="58"/>
+      <c r="B12" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="8">
@@ -3185,12 +3224,16 @@
         <f>IFERROR(VLOOKUP($C12,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala(automatisch, manuell, nicht möglich)</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="46"/>
+      <c r="E12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="35">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="9">
         <v>5</v>
       </c>
@@ -3198,12 +3241,16 @@
         <f>IFERROR(VLOOKUP($C13,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala(automatisch, manuell, nicht möglich)</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="47"/>
+      <c r="E13" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="36">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="9">
         <v>6</v>
       </c>
@@ -3211,97 +3258,117 @@
         <f>IFERROR(VLOOKUP($C14,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (enthalten, leicht umsetzbar, schwer umsetzbar)</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="47"/>
+      <c r="E14" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="str">
         <f>IFERROR(VLOOKUP($C15,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (Verfügbar, leicht umsetzbar, schwer umsetzbar)</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="47"/>
+      <c r="E15" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="9">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="str">
         <f>IFERROR(VLOOKUP($C16,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (Verfügbar, leicht umsetzbar, schwer umsetzbar)</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="47"/>
+      <c r="E16" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="36">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="9">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2" t="str">
         <f>IFERROR(VLOOKUP($C17,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (Verfügbar, leicht umsetzbar, schwer umsetzbar)</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="47"/>
+      <c r="E17" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="36">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="17"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2" t="str">
         <f>IFERROR(VLOOKUP($C18,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (Verfügbar, leicht umsetzbar, schwer umsetzbar)</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="47"/>
+      <c r="E18" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="36">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="9"/>
       <c r="D19" s="2" t="str">
         <f>IFERROR(VLOOKUP($C19,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="47"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="9"/>
       <c r="D20" s="2" t="str">
         <f>IFERROR(VLOOKUP($C20,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="47"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="10"/>
       <c r="D21" s="3" t="str">
         <f>IFERROR(VLOOKUP($C21,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="48"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="16" t="s">
+      <c r="A22" s="58"/>
+      <c r="B22" s="54" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="8">
@@ -3311,12 +3378,16 @@
         <f>IFERROR(VLOOKUP($C22,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (enthalten, leicht umsetzbar, schwer umsetzbar)</v>
       </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="46"/>
+      <c r="E22" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="35">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="9">
         <v>2</v>
       </c>
@@ -3324,12 +3395,16 @@
         <f>IFERROR(VLOOKUP($C23,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (automatisch, manuell, nicht möglich)</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="47"/>
+      <c r="E23" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="36">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="17"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="9">
         <v>3</v>
       </c>
@@ -3337,211 +3412,231 @@
         <f>IFERROR(VLOOKUP($C24,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (automatisch, manuell, nicht möglich)</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="47"/>
+      <c r="E24" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="36">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="17"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="9">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="2" t="str">
         <f>IFERROR(VLOOKUP($C25,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (sehr gut, gut, schlecht)</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="47"/>
+      <c r="E25" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="36">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="9">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2" t="str">
         <f>IFERROR(VLOOKUP($C26,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Ordinalskala (Sehr Umfangreich mit Beispielen, Umfangreich, Einfach, keine)</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="47"/>
+      <c r="E26" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="36">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="9"/>
       <c r="D27" s="2" t="str">
         <f>IFERROR(VLOOKUP($C27,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="47"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="9"/>
       <c r="D28" s="2" t="str">
         <f>IFERROR(VLOOKUP($C28,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="47"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="9"/>
       <c r="D29" s="2" t="str">
         <f>IFERROR(VLOOKUP($C29,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="47"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="36"/>
     </row>
     <row r="30" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="9"/>
       <c r="D30" s="2" t="str">
         <f>IFERROR(VLOOKUP($C30,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="47"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="36"/>
     </row>
     <row r="31" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="18"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="10"/>
       <c r="D31" s="3" t="str">
         <f>IFERROR(VLOOKUP($C31,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="48"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="37"/>
     </row>
     <row r="32" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="54" t="s">
         <v>28</v>
       </c>
       <c r="C32" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" s="1" t="str">
         <f>IFERROR(VLOOKUP($C32,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>LoC</v>
       </c>
-      <c r="E32" s="24"/>
-      <c r="F32" s="46"/>
+      <c r="E32" s="14">
+        <v>45</v>
+      </c>
+      <c r="F32" s="35">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="17"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33" s="2" t="str">
         <f>IFERROR(VLOOKUP($C33,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Methodenaufrufe</v>
       </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="47"/>
+      <c r="E33" s="15">
+        <v>13</v>
+      </c>
+      <c r="F33" s="36">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-      <c r="B34" s="17"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="9"/>
       <c r="D34" s="2" t="str">
         <f>IFERROR(VLOOKUP($C34,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="47"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="36"/>
     </row>
     <row r="35" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="17"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="9"/>
       <c r="D35" s="2" t="str">
         <f>IFERROR(VLOOKUP($C35,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="47"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="36"/>
     </row>
     <row r="36" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
-      <c r="B36" s="17"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="55"/>
       <c r="C36" s="9"/>
       <c r="D36" s="2" t="str">
         <f>IFERROR(VLOOKUP($C36,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="47"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="36"/>
     </row>
     <row r="37" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
-      <c r="B37" s="17"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="55"/>
       <c r="C37" s="9"/>
       <c r="D37" s="2" t="str">
         <f>IFERROR(VLOOKUP($C37,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="47"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="36"/>
     </row>
     <row r="38" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
-      <c r="B38" s="17"/>
+      <c r="A38" s="58"/>
+      <c r="B38" s="55"/>
       <c r="C38" s="9"/>
       <c r="D38" s="2" t="str">
         <f>IFERROR(VLOOKUP($C38,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="47"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="36"/>
     </row>
     <row r="39" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
-      <c r="B39" s="17"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="9"/>
       <c r="D39" s="2" t="str">
         <f>IFERROR(VLOOKUP($C39,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="47"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="36"/>
     </row>
     <row r="40" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
-      <c r="B40" s="17"/>
+      <c r="A40" s="58"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="9"/>
       <c r="D40" s="2" t="str">
         <f>IFERROR(VLOOKUP($C40,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E40" s="25"/>
-      <c r="F40" s="47"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="36"/>
     </row>
     <row r="41" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="18"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="56"/>
       <c r="C41" s="10"/>
       <c r="D41" s="3" t="str">
         <f>IFERROR(VLOOKUP($C41,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E41" s="26"/>
-      <c r="F41" s="48"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="37"/>
     </row>
     <row r="42" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
-      <c r="B42" s="16" t="s">
+      <c r="A42" s="58"/>
+      <c r="B42" s="54" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="8">
@@ -3551,237 +3646,271 @@
         <f>IFERROR(VLOOKUP($C42,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Latenz Antwort bei Messung an Endpunkt ohne Logik</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="46"/>
+      <c r="E42" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" s="35">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="20"/>
-      <c r="B43" s="17"/>
+      <c r="A43" s="58"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="9">
         <v>8</v>
       </c>
       <c r="D43" s="2" t="str">
         <f>IFERROR(VLOOKUP($C43,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
-        <v>Fehlerrate bei 50.000 Anfragen mit 500 echt parallelen Clients in %</v>
-      </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="47"/>
+        <v>Druchsatz bei 100.000 Anfragen mit 255 echt parallelen Clients in Anfragen/Sek</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="55"/>
       <c r="C44" s="9">
         <v>9</v>
       </c>
       <c r="D44" s="2" t="str">
         <f>IFERROR(VLOOKUP($C44,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
-        <v>Druchsatz bei 50.000 Anfragen mit 500 echt parallelen Clients in Anfragen/Sek</v>
-      </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="47"/>
+        <v>Messung Heap Size unter Last: Kleiner 100MB</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="9">
-        <v>10</v>
-      </c>
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="9"/>
       <c r="D45" s="2" t="str">
         <f>IFERROR(VLOOKUP($C45,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
-        <v>Messung Heap Size: Kleiner 100MB</v>
-      </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="47"/>
+        <v/>
+      </c>
+      <c r="E45" s="15"/>
+      <c r="F45" s="36"/>
     </row>
     <row r="46" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="20"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="9"/>
       <c r="D46" s="2" t="str">
         <f>IFERROR(VLOOKUP($C46,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E46" s="25"/>
-      <c r="F46" s="47"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="36"/>
     </row>
     <row r="47" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
-      <c r="B47" s="17"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="9"/>
       <c r="D47" s="2" t="str">
         <f>IFERROR(VLOOKUP($C47,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="47"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="36"/>
     </row>
     <row r="48" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="20"/>
-      <c r="B48" s="17"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="55"/>
       <c r="C48" s="9"/>
       <c r="D48" s="2" t="str">
         <f>IFERROR(VLOOKUP($C48,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E48" s="25"/>
-      <c r="F48" s="47"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="36"/>
     </row>
     <row r="49" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="20"/>
-      <c r="B49" s="17"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="9"/>
       <c r="D49" s="2" t="str">
         <f>IFERROR(VLOOKUP($C49,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E49" s="25"/>
-      <c r="F49" s="47"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="36"/>
     </row>
     <row r="50" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="20"/>
-      <c r="B50" s="17"/>
+      <c r="A50" s="58"/>
+      <c r="B50" s="55"/>
       <c r="C50" s="9"/>
       <c r="D50" s="2" t="str">
         <f>IFERROR(VLOOKUP($C50,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E50" s="25"/>
-      <c r="F50" s="47"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="36"/>
     </row>
     <row r="51" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="18"/>
+      <c r="A51" s="58"/>
+      <c r="B51" s="56"/>
       <c r="C51" s="10"/>
       <c r="D51" s="3" t="str">
         <f>IFERROR(VLOOKUP($C51,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E51" s="26"/>
-      <c r="F51" s="48"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="37"/>
     </row>
     <row r="52" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="20"/>
-      <c r="B52" s="16" t="s">
+      <c r="A52" s="58"/>
+      <c r="B52" s="54" t="s">
         <v>31</v>
       </c>
       <c r="C52" s="8">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D52" s="1" t="str">
         <f>IFERROR(VLOOKUP($C52,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
-        <v>Länge vom Support in Jahren pro Major Release</v>
-      </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="46"/>
+        <v>Länge vom Support in Monaten pro Major Release</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F52" s="35">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="20"/>
-      <c r="B53" s="17"/>
+      <c r="A53" s="58"/>
+      <c r="B53" s="55"/>
       <c r="C53" s="9">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D53" s="2" t="str">
         <f>IFERROR(VLOOKUP($C53,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Kommerzieller Support vorhanden (j/n)</v>
       </c>
-      <c r="E53" s="25"/>
-      <c r="F53" s="47"/>
+      <c r="E53" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F53" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="20"/>
-      <c r="B54" s="17"/>
+      <c r="A54" s="58"/>
+      <c r="B54" s="55"/>
       <c r="C54" s="9">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D54" s="2" t="str">
         <f>IFERROR(VLOOKUP($C54,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Release Zykluslänge bzw. Durchschnittlicher Majorrelease Abstand</v>
       </c>
-      <c r="E54" s="25"/>
-      <c r="F54" s="47"/>
+      <c r="E54" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F54" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="20"/>
-      <c r="B55" s="17"/>
+      <c r="A55" s="58"/>
+      <c r="B55" s="55"/>
       <c r="C55" s="9">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D55" s="2" t="str">
         <f>IFERROR(VLOOKUP($C55,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
-        <v>Anzahl Firmen über 1000 MA</v>
-      </c>
-      <c r="E55" s="25"/>
-      <c r="F55" s="47"/>
+        <v>Firmen über 1000 MA</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F55" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
-      <c r="B56" s="17"/>
+      <c r="A56" s="58"/>
+      <c r="B56" s="55"/>
       <c r="C56" s="9">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D56" s="2" t="str">
         <f>IFERROR(VLOOKUP($C56,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
-        <v>Anzahl Firmen über 100 MA</v>
-      </c>
-      <c r="E56" s="25"/>
-      <c r="F56" s="47"/>
+        <v>Firmen über 100 MA</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="20"/>
-      <c r="B57" s="17"/>
+      <c r="A57" s="58"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="9">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D57" s="2" t="str">
         <f>IFERROR(VLOOKUP($C57,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v>Github - Star + Watch + Fork</v>
       </c>
-      <c r="E57" s="25"/>
-      <c r="F57" s="47"/>
+      <c r="E57" s="15">
+        <v>6850</v>
+      </c>
+      <c r="F57" s="36">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="20"/>
-      <c r="B58" s="17"/>
+      <c r="A58" s="58"/>
+      <c r="B58" s="55"/>
       <c r="C58" s="9"/>
       <c r="D58" s="2" t="str">
         <f>IFERROR(VLOOKUP($C58,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E58" s="25"/>
-      <c r="F58" s="47"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="36"/>
     </row>
     <row r="59" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="20"/>
-      <c r="B59" s="17"/>
+      <c r="A59" s="58"/>
+      <c r="B59" s="55"/>
       <c r="C59" s="9"/>
       <c r="D59" s="2" t="str">
         <f>IFERROR(VLOOKUP($C59,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E59" s="25"/>
-      <c r="F59" s="47"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="36"/>
     </row>
     <row r="60" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="20"/>
-      <c r="B60" s="17"/>
+      <c r="A60" s="58"/>
+      <c r="B60" s="55"/>
       <c r="C60" s="9"/>
       <c r="D60" s="2" t="str">
         <f>IFERROR(VLOOKUP($C60,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E60" s="25"/>
-      <c r="F60" s="47"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="36"/>
     </row>
     <row r="61" spans="1:6" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
-      <c r="B61" s="18"/>
+      <c r="A61" s="59"/>
+      <c r="B61" s="56"/>
       <c r="C61" s="10"/>
       <c r="D61" s="3" t="str">
         <f>IFERROR(VLOOKUP($C61,'QUT-GQM'!F:G,2,FALSE),"")  &amp; ""</f>
         <v/>
       </c>
-      <c r="E61" s="26"/>
-      <c r="F61" s="48"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3803,8 +3932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3813,119 +3942,119 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>42</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7" s="30">
         <f>SUM('QUT-GQM'!H2:H7)</f>
         <v>2.75</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="30">
         <f>SUM('QUT-GQM'!I2:I7)</f>
-        <v>0</v>
+        <v>1.5625</v>
       </c>
       <c r="D7">
         <f>IFERROR(C7/B7,0)</f>
-        <v>0</v>
+        <v>0.56818181818181823</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="41">
-        <f>SUM('QUT-GQM'!H8:H11)</f>
-        <v>1.75</v>
-      </c>
-      <c r="C8" s="41">
-        <f>SUM('QUT-GQM'!I8:I11)</f>
-        <v>0</v>
+      <c r="B8" s="30">
+        <f>SUM('QUT-GQM'!H8:H10)</f>
+        <v>1.25</v>
+      </c>
+      <c r="C8" s="30">
+        <f>SUM('QUT-GQM'!I8:I10)</f>
+        <v>1.25</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D12" si="0">IFERROR(C8/B8,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="41">
-        <f>SUM('QUT-GQM'!H12:H18)</f>
+      <c r="B9" s="30">
+        <f>SUM('QUT-GQM'!H11:H17)</f>
         <v>3.5</v>
       </c>
-      <c r="C9" s="41">
-        <f>SUM('QUT-GQM'!I12:I18)</f>
-        <v>0</v>
+      <c r="C9" s="30">
+        <f>SUM('QUT-GQM'!I11:I17)</f>
+        <v>1.9550000000000001</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.55857142857142861</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="41">
-        <f>SUM('QUT-GQM'!H19:H20)</f>
+      <c r="B10" s="30">
+        <f>SUM('QUT-GQM'!H18:H19)</f>
         <v>1.5</v>
       </c>
-      <c r="C10" s="41">
-        <f>SUM('QUT-GQM'!I19:I20)</f>
-        <v>0</v>
+      <c r="C10" s="30">
+        <f>SUM('QUT-GQM'!I18:I19)</f>
+        <v>0.5</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="41">
-        <f>SUM('QUT-GQM'!H21:H24)</f>
+      <c r="B11" s="30">
+        <f>SUM('QUT-GQM'!H20:H23)</f>
         <v>1.75</v>
       </c>
-      <c r="C11" s="41">
-        <f>SUM('QUT-GQM'!I21:I24)</f>
-        <v>0</v>
+      <c r="C11" s="30">
+        <f>SUM('QUT-GQM'!I20:I23)</f>
+        <v>0.5</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="41">
-        <f>SUM('QUT-GQM'!H25:H28)</f>
+        <v>93</v>
+      </c>
+      <c r="B12" s="30">
+        <f>SUM('QUT-GQM'!H24:H27)</f>
         <v>1.2</v>
       </c>
-      <c r="C12" s="41">
-        <f>SUM('QUT-GQM'!I25:I28)</f>
-        <v>0</v>
+      <c r="C12" s="30">
+        <f>SUM('QUT-GQM'!I24:I27)</f>
+        <v>0.125</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>